<commit_message>
Shoppingbag and ordering stuff
</commit_message>
<xml_diff>
--- a/documenten/Requirements/Requirements.xlsx
+++ b/documenten/Requirements/Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
   <si>
     <t>Als beheerder wil ik producten bewerken zodat de gegevens ervan kloppen.</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Als beheerder wil ik categorieen verwijderen zodat niet meer gebruikte categorieen niet meer in de weg staan.</t>
   </si>
   <si>
-    <t>Als beheerder wil ik de status van een bestelling veranderen naar betaald als het geld van de bestelling is ontvangen om zo duidelijk te maken dat de overdracht is gelukt.</t>
-  </si>
-  <si>
     <t>Als beheerder wil ik de status van een bestelling veranderen naar "Verstuurd" om zo de klant duidelijk te maken dat de bestelling verstuurd is.</t>
   </si>
   <si>
@@ -320,6 +317,21 @@
   </si>
   <si>
     <t>Als gebruiker wil ik meteen kunnen snappen waar ik naartoe moet om een bepaald product te vinden.</t>
+  </si>
+  <si>
+    <t>Als beheerder wil ik de status van een bestelling veranderen naar "Nog niet betaald" om zo de klant duidelijk te maken dat de bestelling nog niet betaald is.</t>
+  </si>
+  <si>
+    <t>Als beheerder wil ik de status van een bestelling veranderen naar "betaald" als het geld van de bestelling is ontvangen om zo duidelijk te maken dat de overdracht is gelukt.</t>
+  </si>
+  <si>
+    <t>Als beheerder wil ik de status van een bestelling veranderen naar "Teruggezonden" om zo de klant duidelijk te maken dat de retour aangekomen is.</t>
+  </si>
+  <si>
+    <t>UR38</t>
+  </si>
+  <si>
+    <t>UR39</t>
   </si>
 </sst>
 </file>
@@ -442,9 +454,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -501,8 +513,35 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -515,8 +554,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="B1:D41" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B1:D41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="B1:D43" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B1:D43"/>
+  <sortState ref="B2:D43">
+    <sortCondition ref="C2"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Beschrijving" dataDxfId="2"/>
     <tableColumn id="2" name="Prioriteit (MoSCoW)" dataDxfId="1"/>
@@ -527,9 +569,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -567,9 +609,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,7 +646,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,7 +681,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -813,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="164.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,660 +870,680 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>79</v>
+      <c r="A41" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>91</v>
+      <c r="A42" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>89</v>
+      <c r="C49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>